<commit_message>
NPeres: v1.10. Dashboard code tested and working after adding reliability graph.
</commit_message>
<xml_diff>
--- a/failures_df_ar.xlsx
+++ b/failures_df_ar.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2575,6 +2575,206 @@
         <v>1825.5</v>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" s="2" t="n">
+        <v>44896.3125</v>
+      </c>
+      <c r="C54" s="2" t="n">
+        <v>44896.33333333334</v>
+      </c>
+      <c r="D54" s="3" t="n">
+        <v>0.02083333333333333</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>t_ar</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>6.764646464646465</v>
+      </c>
+      <c r="G54" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" s="3" t="n">
+        <v>0.02083333333333333</v>
+      </c>
+      <c r="I54" s="3" t="n">
+        <v>0.9791666666666666</v>
+      </c>
+      <c r="J54" s="3" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="K54" s="3" t="n">
+        <v>77.04166666666667</v>
+      </c>
+      <c r="L54" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" s="2" t="n">
+        <v>44897.3125</v>
+      </c>
+      <c r="C55" s="2" t="n">
+        <v>44897.33333333334</v>
+      </c>
+      <c r="D55" s="3" t="n">
+        <v>0.02083333333333333</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>t_ar</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>6.764646464646465</v>
+      </c>
+      <c r="G55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" s="3" t="n">
+        <v>0.02083333333333333</v>
+      </c>
+      <c r="I55" s="3" t="n">
+        <v>3.020833333333333</v>
+      </c>
+      <c r="J55" s="3" t="n">
+        <v>5.770833333333333</v>
+      </c>
+      <c r="K55" s="3" t="n">
+        <v>80.0625</v>
+      </c>
+      <c r="L55" t="n">
+        <v>1921.5</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" s="2" t="n">
+        <v>44900.35416666666</v>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>44900.375</v>
+      </c>
+      <c r="D56" s="3" t="n">
+        <v>0.02083333333333333</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>t_ar</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>6.764646464646465</v>
+      </c>
+      <c r="G56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" s="3" t="n">
+        <v>0.02083333333333333</v>
+      </c>
+      <c r="I56" s="3" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="J56" s="3" t="n">
+        <v>5.791666666666667</v>
+      </c>
+      <c r="K56" s="3" t="n">
+        <v>80.5</v>
+      </c>
+      <c r="L56" t="n">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2" t="n">
+        <v>44900.8125</v>
+      </c>
+      <c r="C57" s="2" t="n">
+        <v>44900.83333333334</v>
+      </c>
+      <c r="D57" s="3" t="n">
+        <v>0.02083333333333333</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>t_ar</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>6.764646464646465</v>
+      </c>
+      <c r="G57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" s="3" t="n">
+        <v>0.02083333333333333</v>
+      </c>
+      <c r="I57" s="3" t="n">
+        <v>0.4791666666666667</v>
+      </c>
+      <c r="J57" s="3" t="n">
+        <v>5.8125</v>
+      </c>
+      <c r="K57" s="3" t="n">
+        <v>80.97916666666667</v>
+      </c>
+      <c r="L57" t="n">
+        <v>1943.5</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" s="2" t="n">
+        <v>44901.3125</v>
+      </c>
+      <c r="C58" s="2" t="n">
+        <v>44901.33333333334</v>
+      </c>
+      <c r="D58" s="3" t="n">
+        <v>0.02083333333333333</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>t_ar</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>6.764646464646465</v>
+      </c>
+      <c r="G58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" s="3" t="n">
+        <v>0.02083333333333333</v>
+      </c>
+      <c r="I58" s="3" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="J58" s="3" t="n">
+        <v>5.833333333333333</v>
+      </c>
+      <c r="K58" s="3" t="n">
+        <v>88.47916666666667</v>
+      </c>
+      <c r="L58" t="n">
+        <v>2123.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>